<commit_message>
excel sheet, graph mapping
</commit_message>
<xml_diff>
--- a/mark59-scripting-samples/mark59serverprofiles.xlsx
+++ b/mark59-scripting-samples/mark59serverprofiles.xlsx
@@ -723,28 +723,28 @@
 Write-Host "FreeDiskSpace["$FreeDiskSpace"]" ;</t>
   </si>
   <si>
-    <t>if ('${PROFILE_SERVER}' -eq 'localhost'){
-    &lt;# Write-Output \"get localhost metric \"; #&gt;
-    $PerfRawData = Get-WmiObject Win32_PerfRawData_PerfOS_System;
-} elseif ((![string]::IsNullOrEmpty('${SECURE_STRING_TXT}')) -and ([string]::IsNullOrEmpty('${SECURE_KEY_ARRAY}'))){
-    &lt;# Write-Output \"  cpu using secure string \"; #&gt;
-    $securePwd = '${SECURE_STRING_TXT}' | ConvertTo-SecureString; 
-    $credential = New-Object System.Management.Automation.PSCredential ('${PROFILE_USERNAME}', $securePwd);
-} elseif ((![string]::IsNullOrEmpty('${SECURE_STRING_TXT}')) -and (![string]::IsNullOrEmpty('${SECURE_KEY_ARRAY}'))){
-    &lt;# Write-Output \"get remote server metric using using secure string with key \"; #&gt;
-    [Byte[]] $key = @(${SECURE_KEY_ARRAY}); 
-    $securePwd = '${SECURE_STRING_TXT}' | ConvertTo-SecureString -Key $key;
-    $credential = New-Object System.Management.Automation.PSCredential ('${PROFILE_USERNAME}', $securePwd);
-} else {
-    &lt;# Write-Output \"get remote server metric using profile username and password \"; #&gt;
-    $password = ConvertTo-SecureString '${PROFILE_PASSWORD}' -AsPlainText -Force; 
-    $credential = New-Object System.Management.Automation.PSCredential ('${PROFILE_USERNAME}', $password);
-}
-if ('${PROFILE_SERVER}' -ne 'localhost'){ 
-    $PerfRawData = Get-WmiObject -Credential $credential -ComputerName ${PROFILE_SERVER} Win32_PerfRawData_PerfOS_System
-}
-$CPUQlen = [math]::round(($PerfRawData | Measure-Object -Property ProcessorQueueLength -Average | Select-Object Average).Average);
-$Processes = [math]::round(($PerfRawData | Measure-Object -Property Processes -Average | Select-Object Average).Average);
+    <t>if ('${PROFILE_SERVER}' -eq 'localhost'){
+    &lt;# Write-Output \"get localhost  metric \"; #&gt;
+    $PerfRawData = Get-WmiObject Win32_PerfRawData_PerfOS_System;
+} elseif ((![string]::IsNullOrEmpty('${SECURE_STRING_TXT}')) -and ([string]::IsNullOrEmpty('${SECURE_KEY_ARRAY}'))){
+    &lt;# Write-Output \"  cpu using secure string \"; #&gt;
+    $securePwd = '${SECURE_STRING_TXT}' | ConvertTo-SecureString; 
+    $credential = New-Object System.Management.Automation.PSCredential ('${PROFILE_USERNAME}', $securePwd);
+} elseif ((![string]::IsNullOrEmpty('${SECURE_STRING_TXT}')) -and (![string]::IsNullOrEmpty('${SECURE_KEY_ARRAY}'))){
+    &lt;# Write-Output \"get remote server metric using using secure string with key \"; #&gt;
+    [Byte[]] $key = @(${SECURE_KEY_ARRAY}); 
+    $securePwd = '${SECURE_STRING_TXT}' | ConvertTo-SecureString -Key $key;
+    $credential = New-Object System.Management.Automation.PSCredential ('${PROFILE_USERNAME}', $securePwd);
+} else {
+    &lt;# Write-Output \"get remote server metric using profile username and password \"; #&gt;
+    $password = ConvertTo-SecureString '${PROFILE_PASSWORD}' -AsPlainText -Force; 
+    $credential = New-Object System.Management.Automation.PSCredential ('${PROFILE_USERNAME}', $password);
+}
+if ('${PROFILE_SERVER}' -ne 'localhost'){ 
+    $PerfRawData = Get-WmiObject -Credential $credential -ComputerName ${PROFILE_SERVER} Win32_PerfRawData_PerfOS_System
+}
+$CPUQlen = [math]::round(($PerfRawData | Measure-Object -Property ProcessorQueueLength -Average | Select-Object Average).Average);
+$Processes = [math]::round(($PerfRawData | Measure-Object -Property Processes -Average | Select-Object Average).Average);
 Write-Host " CPUQlen["$CPUQlen"] Processes["$Processes"] " ;</t>
   </si>
   <si>

</xml_diff>